<commit_message>
Quite major updates to output job file and deliverable capure based on thse files. There are still issues with generation of the DNP list however.
</commit_message>
<xml_diff>
--- a/src/ASSY Config.xlsx
+++ b/src/ASSY Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ASSY Config" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
   <si>
     <t>Encoding:</t>
   </si>
@@ -178,6 +178,114 @@
   </si>
   <si>
     <t>base 30 encoding</t>
+  </si>
+  <si>
+    <t>Bill of Materials</t>
+  </si>
+  <si>
+    <t>BM Raspberry Pi testing interface</t>
+  </si>
+  <si>
+    <t>Part Number:</t>
+  </si>
+  <si>
+    <t>705-02259</t>
+  </si>
+  <si>
+    <t>REV</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>Source Data From:</t>
+  </si>
+  <si>
+    <t>BM Pi Interface.BomDoc</t>
+  </si>
+  <si>
+    <t>Assembly Number:</t>
+  </si>
+  <si>
+    <t>710-02260</t>
+  </si>
+  <si>
+    <t>Total Price:</t>
+  </si>
+  <si>
+    <t>Creation Date:</t>
+  </si>
+  <si>
+    <t>15/07/2020</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>DNP Designators</t>
+  </si>
+  <si>
+    <t>Customer Reference</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Manufacturer 1</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number 1</t>
+  </si>
+  <si>
+    <t>Supplier 1</t>
+  </si>
+  <si>
+    <t>Supplier Part Number 1</t>
+  </si>
+  <si>
+    <t>Manufacturer 2</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number 2</t>
+  </si>
+  <si>
+    <t>Supplier 2</t>
+  </si>
+  <si>
+    <t>Supplier Part Number 2</t>
+  </si>
+  <si>
+    <t>Supplier Subtotal 1</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C6, C7, C8, C9</t>
+  </si>
+  <si>
+    <t>02259A0: C1, C2, C3, C6, C7, C8, C9</t>
+  </si>
+  <si>
+    <t>Capacitor 100nF 0805 X7R 50V 5%</t>
+  </si>
+  <si>
+    <t>Kyocera AVX</t>
+  </si>
+  <si>
+    <t>08055C104JAT2A</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>478-3352-1-ND</t>
+  </si>
+  <si>
+    <t>08051C104JAT2A\2K</t>
+  </si>
+  <si>
+    <t>478-5780-1-ND</t>
   </si>
 </sst>
 </file>
@@ -422,7 +530,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -449,9 +557,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -467,9 +572,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -487,7 +589,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -571,6 +672,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -876,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -921,7 +1041,7 @@
       <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="46" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1496,1555 +1616,1880 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="35.85546875" style="37" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="37" bestFit="1" customWidth="1"/>
-    <col min="12" max="258" width="9.140625" style="37" customWidth="1"/>
-    <col min="259" max="259" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="262" max="264" width="35.85546875" style="37" customWidth="1"/>
-    <col min="265" max="265" width="36.42578125" style="37" customWidth="1"/>
-    <col min="266" max="266" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="268" max="514" width="9.140625" style="37" customWidth="1"/>
-    <col min="515" max="515" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="516" max="516" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="517" max="517" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="518" max="520" width="35.85546875" style="37" customWidth="1"/>
-    <col min="521" max="521" width="36.42578125" style="37" customWidth="1"/>
-    <col min="522" max="522" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="523" max="523" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="524" max="770" width="9.140625" style="37" customWidth="1"/>
-    <col min="771" max="771" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="772" max="772" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="773" max="773" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="774" max="776" width="35.85546875" style="37" customWidth="1"/>
-    <col min="777" max="777" width="36.42578125" style="37" customWidth="1"/>
-    <col min="778" max="778" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="779" max="779" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="780" max="1026" width="9.140625" style="37" customWidth="1"/>
-    <col min="1027" max="1027" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1028" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1029" max="1029" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1030" max="1032" width="35.85546875" style="37" customWidth="1"/>
-    <col min="1033" max="1033" width="36.42578125" style="37" customWidth="1"/>
-    <col min="1034" max="1034" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1035" max="1035" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="1036" max="1282" width="9.140625" style="37" customWidth="1"/>
-    <col min="1283" max="1283" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1284" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1285" max="1285" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1286" max="1288" width="35.85546875" style="37" customWidth="1"/>
-    <col min="1289" max="1289" width="36.42578125" style="37" customWidth="1"/>
-    <col min="1290" max="1290" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1291" max="1291" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="1292" max="1538" width="9.140625" style="37" customWidth="1"/>
-    <col min="1539" max="1539" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1540" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1541" max="1541" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1542" max="1544" width="35.85546875" style="37" customWidth="1"/>
-    <col min="1545" max="1545" width="36.42578125" style="37" customWidth="1"/>
-    <col min="1546" max="1546" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1547" max="1547" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="1548" max="1794" width="9.140625" style="37" customWidth="1"/>
-    <col min="1795" max="1795" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1796" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1797" max="1797" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1798" max="1800" width="35.85546875" style="37" customWidth="1"/>
-    <col min="1801" max="1801" width="36.42578125" style="37" customWidth="1"/>
-    <col min="1802" max="1802" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="1803" max="1803" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="1804" max="2050" width="9.140625" style="37" customWidth="1"/>
-    <col min="2051" max="2051" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2052" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2053" max="2053" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2054" max="2056" width="35.85546875" style="37" customWidth="1"/>
-    <col min="2057" max="2057" width="36.42578125" style="37" customWidth="1"/>
-    <col min="2058" max="2058" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2059" max="2059" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="2060" max="2306" width="9.140625" style="37" customWidth="1"/>
-    <col min="2307" max="2307" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2308" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2309" max="2309" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2310" max="2312" width="35.85546875" style="37" customWidth="1"/>
-    <col min="2313" max="2313" width="36.42578125" style="37" customWidth="1"/>
-    <col min="2314" max="2314" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2315" max="2315" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="2316" max="2562" width="9.140625" style="37" customWidth="1"/>
-    <col min="2563" max="2563" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2564" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2565" max="2565" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2566" max="2568" width="35.85546875" style="37" customWidth="1"/>
-    <col min="2569" max="2569" width="36.42578125" style="37" customWidth="1"/>
-    <col min="2570" max="2570" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2571" max="2571" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="2572" max="2818" width="9.140625" style="37" customWidth="1"/>
-    <col min="2819" max="2819" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2820" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2821" max="2821" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2822" max="2824" width="35.85546875" style="37" customWidth="1"/>
-    <col min="2825" max="2825" width="36.42578125" style="37" customWidth="1"/>
-    <col min="2826" max="2826" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2827" max="2827" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="2828" max="3074" width="9.140625" style="37" customWidth="1"/>
-    <col min="3075" max="3075" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3076" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3077" max="3077" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3078" max="3080" width="35.85546875" style="37" customWidth="1"/>
-    <col min="3081" max="3081" width="36.42578125" style="37" customWidth="1"/>
-    <col min="3082" max="3082" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3083" max="3083" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="3084" max="3330" width="9.140625" style="37" customWidth="1"/>
-    <col min="3331" max="3331" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3332" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3333" max="3333" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3334" max="3336" width="35.85546875" style="37" customWidth="1"/>
-    <col min="3337" max="3337" width="36.42578125" style="37" customWidth="1"/>
-    <col min="3338" max="3338" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3339" max="3339" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="3340" max="3586" width="9.140625" style="37" customWidth="1"/>
-    <col min="3587" max="3587" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3588" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3589" max="3589" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3590" max="3592" width="35.85546875" style="37" customWidth="1"/>
-    <col min="3593" max="3593" width="36.42578125" style="37" customWidth="1"/>
-    <col min="3594" max="3594" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3595" max="3595" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="3596" max="3842" width="9.140625" style="37" customWidth="1"/>
-    <col min="3843" max="3843" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3844" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3845" max="3845" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3846" max="3848" width="35.85546875" style="37" customWidth="1"/>
-    <col min="3849" max="3849" width="36.42578125" style="37" customWidth="1"/>
-    <col min="3850" max="3850" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3851" max="3851" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="3852" max="4098" width="9.140625" style="37" customWidth="1"/>
-    <col min="4099" max="4099" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4100" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4101" max="4101" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4102" max="4104" width="35.85546875" style="37" customWidth="1"/>
-    <col min="4105" max="4105" width="36.42578125" style="37" customWidth="1"/>
-    <col min="4106" max="4106" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4107" max="4107" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="4108" max="4354" width="9.140625" style="37" customWidth="1"/>
-    <col min="4355" max="4355" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4356" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4357" max="4357" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4358" max="4360" width="35.85546875" style="37" customWidth="1"/>
-    <col min="4361" max="4361" width="36.42578125" style="37" customWidth="1"/>
-    <col min="4362" max="4362" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4363" max="4363" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="4364" max="4610" width="9.140625" style="37" customWidth="1"/>
-    <col min="4611" max="4611" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4612" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4613" max="4613" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4614" max="4616" width="35.85546875" style="37" customWidth="1"/>
-    <col min="4617" max="4617" width="36.42578125" style="37" customWidth="1"/>
-    <col min="4618" max="4618" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4619" max="4619" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="4620" max="4866" width="9.140625" style="37" customWidth="1"/>
-    <col min="4867" max="4867" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4868" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4869" max="4869" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4870" max="4872" width="35.85546875" style="37" customWidth="1"/>
-    <col min="4873" max="4873" width="36.42578125" style="37" customWidth="1"/>
-    <col min="4874" max="4874" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4875" max="4875" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="4876" max="5122" width="9.140625" style="37" customWidth="1"/>
-    <col min="5123" max="5123" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5124" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5125" max="5125" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5126" max="5128" width="35.85546875" style="37" customWidth="1"/>
-    <col min="5129" max="5129" width="36.42578125" style="37" customWidth="1"/>
-    <col min="5130" max="5130" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5131" max="5131" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="5132" max="5378" width="9.140625" style="37" customWidth="1"/>
-    <col min="5379" max="5379" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5380" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5381" max="5381" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5382" max="5384" width="35.85546875" style="37" customWidth="1"/>
-    <col min="5385" max="5385" width="36.42578125" style="37" customWidth="1"/>
-    <col min="5386" max="5386" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5387" max="5387" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="5388" max="5634" width="9.140625" style="37" customWidth="1"/>
-    <col min="5635" max="5635" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5636" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5637" max="5637" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5638" max="5640" width="35.85546875" style="37" customWidth="1"/>
-    <col min="5641" max="5641" width="36.42578125" style="37" customWidth="1"/>
-    <col min="5642" max="5642" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5643" max="5643" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="5644" max="5890" width="9.140625" style="37" customWidth="1"/>
-    <col min="5891" max="5891" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5892" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5893" max="5893" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5894" max="5896" width="35.85546875" style="37" customWidth="1"/>
-    <col min="5897" max="5897" width="36.42578125" style="37" customWidth="1"/>
-    <col min="5898" max="5898" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5899" max="5899" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="5900" max="6146" width="9.140625" style="37" customWidth="1"/>
-    <col min="6147" max="6147" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6148" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6149" max="6149" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6150" max="6152" width="35.85546875" style="37" customWidth="1"/>
-    <col min="6153" max="6153" width="36.42578125" style="37" customWidth="1"/>
-    <col min="6154" max="6154" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6155" max="6155" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="6156" max="6402" width="9.140625" style="37" customWidth="1"/>
-    <col min="6403" max="6403" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6404" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6405" max="6405" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6406" max="6408" width="35.85546875" style="37" customWidth="1"/>
-    <col min="6409" max="6409" width="36.42578125" style="37" customWidth="1"/>
-    <col min="6410" max="6410" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6411" max="6411" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="6412" max="6658" width="9.140625" style="37" customWidth="1"/>
-    <col min="6659" max="6659" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6660" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6661" max="6661" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6662" max="6664" width="35.85546875" style="37" customWidth="1"/>
-    <col min="6665" max="6665" width="36.42578125" style="37" customWidth="1"/>
-    <col min="6666" max="6666" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6667" max="6667" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="6668" max="6914" width="9.140625" style="37" customWidth="1"/>
-    <col min="6915" max="6915" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6916" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6917" max="6917" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6918" max="6920" width="35.85546875" style="37" customWidth="1"/>
-    <col min="6921" max="6921" width="36.42578125" style="37" customWidth="1"/>
-    <col min="6922" max="6922" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6923" max="6923" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="6924" max="7170" width="9.140625" style="37" customWidth="1"/>
-    <col min="7171" max="7171" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7172" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7173" max="7173" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7174" max="7176" width="35.85546875" style="37" customWidth="1"/>
-    <col min="7177" max="7177" width="36.42578125" style="37" customWidth="1"/>
-    <col min="7178" max="7178" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7179" max="7179" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="7180" max="7426" width="9.140625" style="37" customWidth="1"/>
-    <col min="7427" max="7427" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7428" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7429" max="7429" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7430" max="7432" width="35.85546875" style="37" customWidth="1"/>
-    <col min="7433" max="7433" width="36.42578125" style="37" customWidth="1"/>
-    <col min="7434" max="7434" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7435" max="7435" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="7436" max="7682" width="9.140625" style="37" customWidth="1"/>
-    <col min="7683" max="7683" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7684" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7685" max="7685" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7686" max="7688" width="35.85546875" style="37" customWidth="1"/>
-    <col min="7689" max="7689" width="36.42578125" style="37" customWidth="1"/>
-    <col min="7690" max="7690" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7691" max="7691" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="7692" max="7938" width="9.140625" style="37" customWidth="1"/>
-    <col min="7939" max="7939" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7940" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7941" max="7941" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7942" max="7944" width="35.85546875" style="37" customWidth="1"/>
-    <col min="7945" max="7945" width="36.42578125" style="37" customWidth="1"/>
-    <col min="7946" max="7946" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="7947" max="7947" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="7948" max="8194" width="9.140625" style="37" customWidth="1"/>
-    <col min="8195" max="8195" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8196" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8197" max="8197" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8198" max="8200" width="35.85546875" style="37" customWidth="1"/>
-    <col min="8201" max="8201" width="36.42578125" style="37" customWidth="1"/>
-    <col min="8202" max="8202" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8203" max="8203" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="8204" max="8450" width="9.140625" style="37" customWidth="1"/>
-    <col min="8451" max="8451" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8452" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8453" max="8453" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8454" max="8456" width="35.85546875" style="37" customWidth="1"/>
-    <col min="8457" max="8457" width="36.42578125" style="37" customWidth="1"/>
-    <col min="8458" max="8458" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8459" max="8459" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="8460" max="8706" width="9.140625" style="37" customWidth="1"/>
-    <col min="8707" max="8707" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8708" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8709" max="8709" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8710" max="8712" width="35.85546875" style="37" customWidth="1"/>
-    <col min="8713" max="8713" width="36.42578125" style="37" customWidth="1"/>
-    <col min="8714" max="8714" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8715" max="8715" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="8716" max="8962" width="9.140625" style="37" customWidth="1"/>
-    <col min="8963" max="8963" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8964" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8965" max="8965" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8966" max="8968" width="35.85546875" style="37" customWidth="1"/>
-    <col min="8969" max="8969" width="36.42578125" style="37" customWidth="1"/>
-    <col min="8970" max="8970" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8971" max="8971" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="8972" max="9218" width="9.140625" style="37" customWidth="1"/>
-    <col min="9219" max="9219" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9220" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9221" max="9221" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9222" max="9224" width="35.85546875" style="37" customWidth="1"/>
-    <col min="9225" max="9225" width="36.42578125" style="37" customWidth="1"/>
-    <col min="9226" max="9226" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9227" max="9227" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="9228" max="9474" width="9.140625" style="37" customWidth="1"/>
-    <col min="9475" max="9475" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9476" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9477" max="9477" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9478" max="9480" width="35.85546875" style="37" customWidth="1"/>
-    <col min="9481" max="9481" width="36.42578125" style="37" customWidth="1"/>
-    <col min="9482" max="9482" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9483" max="9483" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="9484" max="9730" width="9.140625" style="37" customWidth="1"/>
-    <col min="9731" max="9731" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9732" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9733" max="9733" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9734" max="9736" width="35.85546875" style="37" customWidth="1"/>
-    <col min="9737" max="9737" width="36.42578125" style="37" customWidth="1"/>
-    <col min="9738" max="9738" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9739" max="9739" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="9740" max="9986" width="9.140625" style="37" customWidth="1"/>
-    <col min="9987" max="9987" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9988" max="9988" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9989" max="9989" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9990" max="9992" width="35.85546875" style="37" customWidth="1"/>
-    <col min="9993" max="9993" width="36.42578125" style="37" customWidth="1"/>
-    <col min="9994" max="9994" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="9995" max="9995" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="9996" max="10242" width="9.140625" style="37" customWidth="1"/>
-    <col min="10243" max="10243" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10244" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10245" max="10245" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10246" max="10248" width="35.85546875" style="37" customWidth="1"/>
-    <col min="10249" max="10249" width="36.42578125" style="37" customWidth="1"/>
-    <col min="10250" max="10250" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10251" max="10251" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="10252" max="10498" width="9.140625" style="37" customWidth="1"/>
-    <col min="10499" max="10499" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10500" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10501" max="10501" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10502" max="10504" width="35.85546875" style="37" customWidth="1"/>
-    <col min="10505" max="10505" width="36.42578125" style="37" customWidth="1"/>
-    <col min="10506" max="10506" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10507" max="10507" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="10508" max="10754" width="9.140625" style="37" customWidth="1"/>
-    <col min="10755" max="10755" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10756" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10757" max="10757" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10758" max="10760" width="35.85546875" style="37" customWidth="1"/>
-    <col min="10761" max="10761" width="36.42578125" style="37" customWidth="1"/>
-    <col min="10762" max="10762" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10763" max="10763" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="10764" max="11010" width="9.140625" style="37" customWidth="1"/>
-    <col min="11011" max="11011" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11012" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11013" max="11013" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11014" max="11016" width="35.85546875" style="37" customWidth="1"/>
-    <col min="11017" max="11017" width="36.42578125" style="37" customWidth="1"/>
-    <col min="11018" max="11018" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11019" max="11019" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="11020" max="11266" width="9.140625" style="37" customWidth="1"/>
-    <col min="11267" max="11267" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11268" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11269" max="11269" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11270" max="11272" width="35.85546875" style="37" customWidth="1"/>
-    <col min="11273" max="11273" width="36.42578125" style="37" customWidth="1"/>
-    <col min="11274" max="11274" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11275" max="11275" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="11276" max="11522" width="9.140625" style="37" customWidth="1"/>
-    <col min="11523" max="11523" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11524" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11525" max="11525" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11526" max="11528" width="35.85546875" style="37" customWidth="1"/>
-    <col min="11529" max="11529" width="36.42578125" style="37" customWidth="1"/>
-    <col min="11530" max="11530" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11531" max="11531" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="11532" max="11778" width="9.140625" style="37" customWidth="1"/>
-    <col min="11779" max="11779" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11780" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11781" max="11781" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11782" max="11784" width="35.85546875" style="37" customWidth="1"/>
-    <col min="11785" max="11785" width="36.42578125" style="37" customWidth="1"/>
-    <col min="11786" max="11786" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11787" max="11787" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="11788" max="12034" width="9.140625" style="37" customWidth="1"/>
-    <col min="12035" max="12035" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12036" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12037" max="12037" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12038" max="12040" width="35.85546875" style="37" customWidth="1"/>
-    <col min="12041" max="12041" width="36.42578125" style="37" customWidth="1"/>
-    <col min="12042" max="12042" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12043" max="12043" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="12044" max="12290" width="9.140625" style="37" customWidth="1"/>
-    <col min="12291" max="12291" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12292" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12293" max="12293" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12294" max="12296" width="35.85546875" style="37" customWidth="1"/>
-    <col min="12297" max="12297" width="36.42578125" style="37" customWidth="1"/>
-    <col min="12298" max="12298" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12299" max="12299" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="12300" max="12546" width="9.140625" style="37" customWidth="1"/>
-    <col min="12547" max="12547" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12548" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12549" max="12549" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12550" max="12552" width="35.85546875" style="37" customWidth="1"/>
-    <col min="12553" max="12553" width="36.42578125" style="37" customWidth="1"/>
-    <col min="12554" max="12554" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12555" max="12555" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="12556" max="12802" width="9.140625" style="37" customWidth="1"/>
-    <col min="12803" max="12803" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12804" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12805" max="12805" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12806" max="12808" width="35.85546875" style="37" customWidth="1"/>
-    <col min="12809" max="12809" width="36.42578125" style="37" customWidth="1"/>
-    <col min="12810" max="12810" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12811" max="12811" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="12812" max="13058" width="9.140625" style="37" customWidth="1"/>
-    <col min="13059" max="13059" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13060" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13061" max="13061" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13062" max="13064" width="35.85546875" style="37" customWidth="1"/>
-    <col min="13065" max="13065" width="36.42578125" style="37" customWidth="1"/>
-    <col min="13066" max="13066" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13067" max="13067" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="13068" max="13314" width="9.140625" style="37" customWidth="1"/>
-    <col min="13315" max="13315" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13316" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13317" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13318" max="13320" width="35.85546875" style="37" customWidth="1"/>
-    <col min="13321" max="13321" width="36.42578125" style="37" customWidth="1"/>
-    <col min="13322" max="13322" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13323" max="13323" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="13324" max="13570" width="9.140625" style="37" customWidth="1"/>
-    <col min="13571" max="13571" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13572" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13573" max="13573" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13574" max="13576" width="35.85546875" style="37" customWidth="1"/>
-    <col min="13577" max="13577" width="36.42578125" style="37" customWidth="1"/>
-    <col min="13578" max="13578" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13579" max="13579" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="13580" max="13826" width="9.140625" style="37" customWidth="1"/>
-    <col min="13827" max="13827" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13828" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13829" max="13829" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13830" max="13832" width="35.85546875" style="37" customWidth="1"/>
-    <col min="13833" max="13833" width="36.42578125" style="37" customWidth="1"/>
-    <col min="13834" max="13834" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13835" max="13835" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="13836" max="14082" width="9.140625" style="37" customWidth="1"/>
-    <col min="14083" max="14083" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14084" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14085" max="14085" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14086" max="14088" width="35.85546875" style="37" customWidth="1"/>
-    <col min="14089" max="14089" width="36.42578125" style="37" customWidth="1"/>
-    <col min="14090" max="14090" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14091" max="14091" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="14092" max="14338" width="9.140625" style="37" customWidth="1"/>
-    <col min="14339" max="14339" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14340" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14341" max="14341" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14342" max="14344" width="35.85546875" style="37" customWidth="1"/>
-    <col min="14345" max="14345" width="36.42578125" style="37" customWidth="1"/>
-    <col min="14346" max="14346" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14347" max="14347" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="14348" max="14594" width="9.140625" style="37" customWidth="1"/>
-    <col min="14595" max="14595" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14596" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14597" max="14597" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14598" max="14600" width="35.85546875" style="37" customWidth="1"/>
-    <col min="14601" max="14601" width="36.42578125" style="37" customWidth="1"/>
-    <col min="14602" max="14602" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14603" max="14603" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="14604" max="14850" width="9.140625" style="37" customWidth="1"/>
-    <col min="14851" max="14851" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14852" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14853" max="14853" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14854" max="14856" width="35.85546875" style="37" customWidth="1"/>
-    <col min="14857" max="14857" width="36.42578125" style="37" customWidth="1"/>
-    <col min="14858" max="14858" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="14859" max="14859" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="14860" max="15106" width="9.140625" style="37" customWidth="1"/>
-    <col min="15107" max="15107" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15108" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15109" max="15109" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15110" max="15112" width="35.85546875" style="37" customWidth="1"/>
-    <col min="15113" max="15113" width="36.42578125" style="37" customWidth="1"/>
-    <col min="15114" max="15114" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15115" max="15115" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="15116" max="15362" width="9.140625" style="37" customWidth="1"/>
-    <col min="15363" max="15363" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15364" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15365" max="15365" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15366" max="15368" width="35.85546875" style="37" customWidth="1"/>
-    <col min="15369" max="15369" width="36.42578125" style="37" customWidth="1"/>
-    <col min="15370" max="15370" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15371" max="15371" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="15372" max="15618" width="9.140625" style="37" customWidth="1"/>
-    <col min="15619" max="15619" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15620" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15621" max="15621" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15622" max="15624" width="35.85546875" style="37" customWidth="1"/>
-    <col min="15625" max="15625" width="36.42578125" style="37" customWidth="1"/>
-    <col min="15626" max="15626" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15627" max="15627" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="15628" max="15874" width="9.140625" style="37" customWidth="1"/>
-    <col min="15875" max="15875" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15876" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15877" max="15877" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15878" max="15880" width="35.85546875" style="37" customWidth="1"/>
-    <col min="15881" max="15881" width="36.42578125" style="37" customWidth="1"/>
-    <col min="15882" max="15882" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="15883" max="15883" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="15884" max="16130" width="9.140625" style="37" customWidth="1"/>
-    <col min="16131" max="16131" width="37.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16132" width="26.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="16133" max="16133" width="34.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="16134" max="16136" width="35.85546875" style="37" customWidth="1"/>
-    <col min="16137" max="16137" width="36.42578125" style="37" customWidth="1"/>
-    <col min="16138" max="16138" width="27.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="16139" max="16139" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="16140" max="16384" width="9.140625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" style="34" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="34" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" style="34" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="34" customWidth="1"/>
+    <col min="11" max="11" width="30.85546875" style="34" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="34" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" style="34" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" style="34" customWidth="1"/>
+    <col min="15" max="261" width="9.140625" style="34" customWidth="1"/>
+    <col min="262" max="262" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="265" max="267" width="35.85546875" style="34" customWidth="1"/>
+    <col min="268" max="268" width="36.42578125" style="34" customWidth="1"/>
+    <col min="269" max="269" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="271" max="517" width="9.140625" style="34" customWidth="1"/>
+    <col min="518" max="518" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="519" max="519" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="521" max="523" width="35.85546875" style="34" customWidth="1"/>
+    <col min="524" max="524" width="36.42578125" style="34" customWidth="1"/>
+    <col min="525" max="525" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="526" max="526" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="527" max="773" width="9.140625" style="34" customWidth="1"/>
+    <col min="774" max="774" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="775" max="775" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="777" max="779" width="35.85546875" style="34" customWidth="1"/>
+    <col min="780" max="780" width="36.42578125" style="34" customWidth="1"/>
+    <col min="781" max="781" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="782" max="782" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="783" max="1029" width="9.140625" style="34" customWidth="1"/>
+    <col min="1030" max="1030" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1031" max="1031" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1033" max="1035" width="35.85546875" style="34" customWidth="1"/>
+    <col min="1036" max="1036" width="36.42578125" style="34" customWidth="1"/>
+    <col min="1037" max="1037" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1038" max="1038" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="1039" max="1285" width="9.140625" style="34" customWidth="1"/>
+    <col min="1286" max="1286" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1287" max="1287" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1289" max="1291" width="35.85546875" style="34" customWidth="1"/>
+    <col min="1292" max="1292" width="36.42578125" style="34" customWidth="1"/>
+    <col min="1293" max="1293" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1294" max="1294" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="1295" max="1541" width="9.140625" style="34" customWidth="1"/>
+    <col min="1542" max="1542" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1543" max="1543" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1545" max="1547" width="35.85546875" style="34" customWidth="1"/>
+    <col min="1548" max="1548" width="36.42578125" style="34" customWidth="1"/>
+    <col min="1549" max="1549" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1550" max="1550" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="1551" max="1797" width="9.140625" style="34" customWidth="1"/>
+    <col min="1798" max="1798" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1799" max="1799" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1801" max="1803" width="35.85546875" style="34" customWidth="1"/>
+    <col min="1804" max="1804" width="36.42578125" style="34" customWidth="1"/>
+    <col min="1805" max="1805" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="1806" max="1806" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="1807" max="2053" width="9.140625" style="34" customWidth="1"/>
+    <col min="2054" max="2054" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2055" max="2055" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2057" max="2059" width="35.85546875" style="34" customWidth="1"/>
+    <col min="2060" max="2060" width="36.42578125" style="34" customWidth="1"/>
+    <col min="2061" max="2061" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2062" max="2062" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="2063" max="2309" width="9.140625" style="34" customWidth="1"/>
+    <col min="2310" max="2310" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2311" max="2311" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2313" max="2315" width="35.85546875" style="34" customWidth="1"/>
+    <col min="2316" max="2316" width="36.42578125" style="34" customWidth="1"/>
+    <col min="2317" max="2317" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2318" max="2318" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="2319" max="2565" width="9.140625" style="34" customWidth="1"/>
+    <col min="2566" max="2566" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2567" max="2567" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2569" max="2571" width="35.85546875" style="34" customWidth="1"/>
+    <col min="2572" max="2572" width="36.42578125" style="34" customWidth="1"/>
+    <col min="2573" max="2573" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2574" max="2574" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="2575" max="2821" width="9.140625" style="34" customWidth="1"/>
+    <col min="2822" max="2822" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2823" max="2823" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2825" max="2827" width="35.85546875" style="34" customWidth="1"/>
+    <col min="2828" max="2828" width="36.42578125" style="34" customWidth="1"/>
+    <col min="2829" max="2829" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2830" max="2830" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="2831" max="3077" width="9.140625" style="34" customWidth="1"/>
+    <col min="3078" max="3078" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3079" max="3079" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3081" max="3083" width="35.85546875" style="34" customWidth="1"/>
+    <col min="3084" max="3084" width="36.42578125" style="34" customWidth="1"/>
+    <col min="3085" max="3085" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3086" max="3086" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="3087" max="3333" width="9.140625" style="34" customWidth="1"/>
+    <col min="3334" max="3334" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3335" max="3335" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3337" max="3339" width="35.85546875" style="34" customWidth="1"/>
+    <col min="3340" max="3340" width="36.42578125" style="34" customWidth="1"/>
+    <col min="3341" max="3341" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3342" max="3342" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="3343" max="3589" width="9.140625" style="34" customWidth="1"/>
+    <col min="3590" max="3590" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3591" max="3591" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3593" max="3595" width="35.85546875" style="34" customWidth="1"/>
+    <col min="3596" max="3596" width="36.42578125" style="34" customWidth="1"/>
+    <col min="3597" max="3597" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3598" max="3598" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="3599" max="3845" width="9.140625" style="34" customWidth="1"/>
+    <col min="3846" max="3846" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3847" max="3847" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3849" max="3851" width="35.85546875" style="34" customWidth="1"/>
+    <col min="3852" max="3852" width="36.42578125" style="34" customWidth="1"/>
+    <col min="3853" max="3853" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3854" max="3854" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="3855" max="4101" width="9.140625" style="34" customWidth="1"/>
+    <col min="4102" max="4102" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4103" max="4103" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4105" max="4107" width="35.85546875" style="34" customWidth="1"/>
+    <col min="4108" max="4108" width="36.42578125" style="34" customWidth="1"/>
+    <col min="4109" max="4109" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4110" max="4110" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="4111" max="4357" width="9.140625" style="34" customWidth="1"/>
+    <col min="4358" max="4358" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4359" max="4359" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4361" max="4363" width="35.85546875" style="34" customWidth="1"/>
+    <col min="4364" max="4364" width="36.42578125" style="34" customWidth="1"/>
+    <col min="4365" max="4365" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4366" max="4366" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="4367" max="4613" width="9.140625" style="34" customWidth="1"/>
+    <col min="4614" max="4614" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4615" max="4615" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4617" max="4619" width="35.85546875" style="34" customWidth="1"/>
+    <col min="4620" max="4620" width="36.42578125" style="34" customWidth="1"/>
+    <col min="4621" max="4621" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4622" max="4622" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="4623" max="4869" width="9.140625" style="34" customWidth="1"/>
+    <col min="4870" max="4870" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4871" max="4871" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4873" max="4875" width="35.85546875" style="34" customWidth="1"/>
+    <col min="4876" max="4876" width="36.42578125" style="34" customWidth="1"/>
+    <col min="4877" max="4877" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4878" max="4878" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="4879" max="5125" width="9.140625" style="34" customWidth="1"/>
+    <col min="5126" max="5126" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5127" max="5127" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5129" max="5131" width="35.85546875" style="34" customWidth="1"/>
+    <col min="5132" max="5132" width="36.42578125" style="34" customWidth="1"/>
+    <col min="5133" max="5133" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5134" max="5134" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="5135" max="5381" width="9.140625" style="34" customWidth="1"/>
+    <col min="5382" max="5382" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5383" max="5383" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5385" max="5387" width="35.85546875" style="34" customWidth="1"/>
+    <col min="5388" max="5388" width="36.42578125" style="34" customWidth="1"/>
+    <col min="5389" max="5389" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5390" max="5390" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="5391" max="5637" width="9.140625" style="34" customWidth="1"/>
+    <col min="5638" max="5638" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5639" max="5639" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5641" max="5643" width="35.85546875" style="34" customWidth="1"/>
+    <col min="5644" max="5644" width="36.42578125" style="34" customWidth="1"/>
+    <col min="5645" max="5645" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5646" max="5646" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="5647" max="5893" width="9.140625" style="34" customWidth="1"/>
+    <col min="5894" max="5894" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5895" max="5895" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5897" max="5899" width="35.85546875" style="34" customWidth="1"/>
+    <col min="5900" max="5900" width="36.42578125" style="34" customWidth="1"/>
+    <col min="5901" max="5901" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5902" max="5902" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="5903" max="6149" width="9.140625" style="34" customWidth="1"/>
+    <col min="6150" max="6150" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6151" max="6151" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6153" max="6155" width="35.85546875" style="34" customWidth="1"/>
+    <col min="6156" max="6156" width="36.42578125" style="34" customWidth="1"/>
+    <col min="6157" max="6157" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6158" max="6158" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="6159" max="6405" width="9.140625" style="34" customWidth="1"/>
+    <col min="6406" max="6406" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6407" max="6407" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6409" max="6411" width="35.85546875" style="34" customWidth="1"/>
+    <col min="6412" max="6412" width="36.42578125" style="34" customWidth="1"/>
+    <col min="6413" max="6413" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6414" max="6414" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="6415" max="6661" width="9.140625" style="34" customWidth="1"/>
+    <col min="6662" max="6662" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6663" max="6663" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6665" max="6667" width="35.85546875" style="34" customWidth="1"/>
+    <col min="6668" max="6668" width="36.42578125" style="34" customWidth="1"/>
+    <col min="6669" max="6669" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6670" max="6670" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="6671" max="6917" width="9.140625" style="34" customWidth="1"/>
+    <col min="6918" max="6918" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6919" max="6919" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6921" max="6923" width="35.85546875" style="34" customWidth="1"/>
+    <col min="6924" max="6924" width="36.42578125" style="34" customWidth="1"/>
+    <col min="6925" max="6925" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6926" max="6926" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="6927" max="7173" width="9.140625" style="34" customWidth="1"/>
+    <col min="7174" max="7174" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7175" max="7175" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7177" max="7179" width="35.85546875" style="34" customWidth="1"/>
+    <col min="7180" max="7180" width="36.42578125" style="34" customWidth="1"/>
+    <col min="7181" max="7181" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7182" max="7182" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="7183" max="7429" width="9.140625" style="34" customWidth="1"/>
+    <col min="7430" max="7430" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7431" max="7431" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7433" max="7435" width="35.85546875" style="34" customWidth="1"/>
+    <col min="7436" max="7436" width="36.42578125" style="34" customWidth="1"/>
+    <col min="7437" max="7437" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7438" max="7438" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="7439" max="7685" width="9.140625" style="34" customWidth="1"/>
+    <col min="7686" max="7686" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7687" max="7687" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7689" max="7691" width="35.85546875" style="34" customWidth="1"/>
+    <col min="7692" max="7692" width="36.42578125" style="34" customWidth="1"/>
+    <col min="7693" max="7693" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7694" max="7694" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="7695" max="7941" width="9.140625" style="34" customWidth="1"/>
+    <col min="7942" max="7942" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7943" max="7943" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7945" max="7947" width="35.85546875" style="34" customWidth="1"/>
+    <col min="7948" max="7948" width="36.42578125" style="34" customWidth="1"/>
+    <col min="7949" max="7949" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7950" max="7950" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="7951" max="8197" width="9.140625" style="34" customWidth="1"/>
+    <col min="8198" max="8198" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8199" max="8199" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8201" max="8203" width="35.85546875" style="34" customWidth="1"/>
+    <col min="8204" max="8204" width="36.42578125" style="34" customWidth="1"/>
+    <col min="8205" max="8205" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8206" max="8206" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="8207" max="8453" width="9.140625" style="34" customWidth="1"/>
+    <col min="8454" max="8454" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8455" max="8455" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8457" max="8459" width="35.85546875" style="34" customWidth="1"/>
+    <col min="8460" max="8460" width="36.42578125" style="34" customWidth="1"/>
+    <col min="8461" max="8461" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8462" max="8462" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="8463" max="8709" width="9.140625" style="34" customWidth="1"/>
+    <col min="8710" max="8710" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8711" max="8711" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8713" max="8715" width="35.85546875" style="34" customWidth="1"/>
+    <col min="8716" max="8716" width="36.42578125" style="34" customWidth="1"/>
+    <col min="8717" max="8717" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8718" max="8718" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="8719" max="8965" width="9.140625" style="34" customWidth="1"/>
+    <col min="8966" max="8966" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8967" max="8967" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8969" max="8971" width="35.85546875" style="34" customWidth="1"/>
+    <col min="8972" max="8972" width="36.42578125" style="34" customWidth="1"/>
+    <col min="8973" max="8973" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8974" max="8974" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="8975" max="9221" width="9.140625" style="34" customWidth="1"/>
+    <col min="9222" max="9222" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9223" max="9223" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9225" max="9227" width="35.85546875" style="34" customWidth="1"/>
+    <col min="9228" max="9228" width="36.42578125" style="34" customWidth="1"/>
+    <col min="9229" max="9229" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9230" max="9230" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="9231" max="9477" width="9.140625" style="34" customWidth="1"/>
+    <col min="9478" max="9478" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9479" max="9479" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9481" max="9483" width="35.85546875" style="34" customWidth="1"/>
+    <col min="9484" max="9484" width="36.42578125" style="34" customWidth="1"/>
+    <col min="9485" max="9485" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9486" max="9486" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="9487" max="9733" width="9.140625" style="34" customWidth="1"/>
+    <col min="9734" max="9734" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9735" max="9735" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9737" max="9739" width="35.85546875" style="34" customWidth="1"/>
+    <col min="9740" max="9740" width="36.42578125" style="34" customWidth="1"/>
+    <col min="9741" max="9741" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9742" max="9742" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="9743" max="9989" width="9.140625" style="34" customWidth="1"/>
+    <col min="9990" max="9990" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9991" max="9991" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9993" max="9995" width="35.85546875" style="34" customWidth="1"/>
+    <col min="9996" max="9996" width="36.42578125" style="34" customWidth="1"/>
+    <col min="9997" max="9997" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9998" max="9998" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="9999" max="10245" width="9.140625" style="34" customWidth="1"/>
+    <col min="10246" max="10246" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10247" max="10247" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10249" max="10251" width="35.85546875" style="34" customWidth="1"/>
+    <col min="10252" max="10252" width="36.42578125" style="34" customWidth="1"/>
+    <col min="10253" max="10253" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10254" max="10254" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="10255" max="10501" width="9.140625" style="34" customWidth="1"/>
+    <col min="10502" max="10502" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10503" max="10503" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10505" max="10507" width="35.85546875" style="34" customWidth="1"/>
+    <col min="10508" max="10508" width="36.42578125" style="34" customWidth="1"/>
+    <col min="10509" max="10509" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10510" max="10510" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="10511" max="10757" width="9.140625" style="34" customWidth="1"/>
+    <col min="10758" max="10758" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10759" max="10759" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10761" max="10763" width="35.85546875" style="34" customWidth="1"/>
+    <col min="10764" max="10764" width="36.42578125" style="34" customWidth="1"/>
+    <col min="10765" max="10765" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10766" max="10766" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="10767" max="11013" width="9.140625" style="34" customWidth="1"/>
+    <col min="11014" max="11014" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11015" max="11015" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11017" max="11019" width="35.85546875" style="34" customWidth="1"/>
+    <col min="11020" max="11020" width="36.42578125" style="34" customWidth="1"/>
+    <col min="11021" max="11021" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11022" max="11022" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="11023" max="11269" width="9.140625" style="34" customWidth="1"/>
+    <col min="11270" max="11270" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11271" max="11271" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11273" max="11275" width="35.85546875" style="34" customWidth="1"/>
+    <col min="11276" max="11276" width="36.42578125" style="34" customWidth="1"/>
+    <col min="11277" max="11277" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11278" max="11278" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="11279" max="11525" width="9.140625" style="34" customWidth="1"/>
+    <col min="11526" max="11526" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11527" max="11527" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11529" max="11531" width="35.85546875" style="34" customWidth="1"/>
+    <col min="11532" max="11532" width="36.42578125" style="34" customWidth="1"/>
+    <col min="11533" max="11533" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11534" max="11534" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="11535" max="11781" width="9.140625" style="34" customWidth="1"/>
+    <col min="11782" max="11782" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11783" max="11783" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11785" max="11787" width="35.85546875" style="34" customWidth="1"/>
+    <col min="11788" max="11788" width="36.42578125" style="34" customWidth="1"/>
+    <col min="11789" max="11789" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11790" max="11790" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="11791" max="12037" width="9.140625" style="34" customWidth="1"/>
+    <col min="12038" max="12038" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12039" max="12039" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12041" max="12043" width="35.85546875" style="34" customWidth="1"/>
+    <col min="12044" max="12044" width="36.42578125" style="34" customWidth="1"/>
+    <col min="12045" max="12045" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12046" max="12046" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="12047" max="12293" width="9.140625" style="34" customWidth="1"/>
+    <col min="12294" max="12294" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12295" max="12295" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12297" max="12299" width="35.85546875" style="34" customWidth="1"/>
+    <col min="12300" max="12300" width="36.42578125" style="34" customWidth="1"/>
+    <col min="12301" max="12301" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12302" max="12302" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="12303" max="12549" width="9.140625" style="34" customWidth="1"/>
+    <col min="12550" max="12550" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12551" max="12551" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12553" max="12555" width="35.85546875" style="34" customWidth="1"/>
+    <col min="12556" max="12556" width="36.42578125" style="34" customWidth="1"/>
+    <col min="12557" max="12557" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12558" max="12558" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="12559" max="12805" width="9.140625" style="34" customWidth="1"/>
+    <col min="12806" max="12806" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12807" max="12807" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12809" max="12811" width="35.85546875" style="34" customWidth="1"/>
+    <col min="12812" max="12812" width="36.42578125" style="34" customWidth="1"/>
+    <col min="12813" max="12813" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12814" max="12814" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="12815" max="13061" width="9.140625" style="34" customWidth="1"/>
+    <col min="13062" max="13062" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13063" max="13063" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13065" max="13067" width="35.85546875" style="34" customWidth="1"/>
+    <col min="13068" max="13068" width="36.42578125" style="34" customWidth="1"/>
+    <col min="13069" max="13069" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13070" max="13070" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="13071" max="13317" width="9.140625" style="34" customWidth="1"/>
+    <col min="13318" max="13318" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13319" max="13319" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13321" max="13323" width="35.85546875" style="34" customWidth="1"/>
+    <col min="13324" max="13324" width="36.42578125" style="34" customWidth="1"/>
+    <col min="13325" max="13325" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13326" max="13326" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="13327" max="13573" width="9.140625" style="34" customWidth="1"/>
+    <col min="13574" max="13574" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13575" max="13575" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13577" max="13579" width="35.85546875" style="34" customWidth="1"/>
+    <col min="13580" max="13580" width="36.42578125" style="34" customWidth="1"/>
+    <col min="13581" max="13581" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13582" max="13582" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="13583" max="13829" width="9.140625" style="34" customWidth="1"/>
+    <col min="13830" max="13830" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13831" max="13831" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13833" max="13835" width="35.85546875" style="34" customWidth="1"/>
+    <col min="13836" max="13836" width="36.42578125" style="34" customWidth="1"/>
+    <col min="13837" max="13837" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13838" max="13838" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="13839" max="14085" width="9.140625" style="34" customWidth="1"/>
+    <col min="14086" max="14086" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14087" max="14087" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14089" max="14091" width="35.85546875" style="34" customWidth="1"/>
+    <col min="14092" max="14092" width="36.42578125" style="34" customWidth="1"/>
+    <col min="14093" max="14093" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14094" max="14094" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="14095" max="14341" width="9.140625" style="34" customWidth="1"/>
+    <col min="14342" max="14342" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14343" max="14343" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14345" max="14347" width="35.85546875" style="34" customWidth="1"/>
+    <col min="14348" max="14348" width="36.42578125" style="34" customWidth="1"/>
+    <col min="14349" max="14349" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14350" max="14350" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="14351" max="14597" width="9.140625" style="34" customWidth="1"/>
+    <col min="14598" max="14598" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14599" max="14599" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14601" max="14603" width="35.85546875" style="34" customWidth="1"/>
+    <col min="14604" max="14604" width="36.42578125" style="34" customWidth="1"/>
+    <col min="14605" max="14605" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14606" max="14606" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="14607" max="14853" width="9.140625" style="34" customWidth="1"/>
+    <col min="14854" max="14854" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14855" max="14855" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14857" max="14859" width="35.85546875" style="34" customWidth="1"/>
+    <col min="14860" max="14860" width="36.42578125" style="34" customWidth="1"/>
+    <col min="14861" max="14861" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14862" max="14862" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="14863" max="15109" width="9.140625" style="34" customWidth="1"/>
+    <col min="15110" max="15110" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15111" max="15111" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15113" max="15115" width="35.85546875" style="34" customWidth="1"/>
+    <col min="15116" max="15116" width="36.42578125" style="34" customWidth="1"/>
+    <col min="15117" max="15117" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15118" max="15118" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="15119" max="15365" width="9.140625" style="34" customWidth="1"/>
+    <col min="15366" max="15366" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15367" max="15367" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15369" max="15371" width="35.85546875" style="34" customWidth="1"/>
+    <col min="15372" max="15372" width="36.42578125" style="34" customWidth="1"/>
+    <col min="15373" max="15373" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15374" max="15374" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="15375" max="15621" width="9.140625" style="34" customWidth="1"/>
+    <col min="15622" max="15622" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15623" max="15623" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15625" max="15627" width="35.85546875" style="34" customWidth="1"/>
+    <col min="15628" max="15628" width="36.42578125" style="34" customWidth="1"/>
+    <col min="15629" max="15629" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15630" max="15630" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="15631" max="15877" width="9.140625" style="34" customWidth="1"/>
+    <col min="15878" max="15878" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15879" max="15879" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15881" max="15883" width="35.85546875" style="34" customWidth="1"/>
+    <col min="15884" max="15884" width="36.42578125" style="34" customWidth="1"/>
+    <col min="15885" max="15885" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15886" max="15886" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="15887" max="16133" width="9.140625" style="34" customWidth="1"/>
+    <col min="16134" max="16134" width="37.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="16135" max="16135" width="26.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="34.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="16137" max="16139" width="35.85546875" style="34" customWidth="1"/>
+    <col min="16140" max="16140" width="36.42578125" style="34" customWidth="1"/>
+    <col min="16141" max="16141" width="27.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="16142" max="16142" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="16143" max="16384" width="9.140625" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="15"/>
-    </row>
-    <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2"/>
-      <c r="K2" s="21"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+    <row r="1" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="58">
+        <v>59.59</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="19"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="28"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
       <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5" s="31"/>
-    </row>
-    <row r="6" spans="1:11" s="34" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-    </row>
-    <row r="7" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="55"/>
-    </row>
-    <row r="8" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="55"/>
-    </row>
-    <row r="9" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="55"/>
-    </row>
-    <row r="10" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="55"/>
-    </row>
-    <row r="11" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55"/>
-    </row>
-    <row r="12" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="55"/>
-    </row>
-    <row r="13" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="55"/>
-    </row>
-    <row r="14" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="55"/>
-    </row>
-    <row r="15" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="55"/>
-    </row>
-    <row r="16" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="55"/>
-    </row>
-    <row r="17" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="55"/>
-    </row>
-    <row r="18" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="55"/>
-    </row>
-    <row r="19" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="55"/>
-    </row>
-    <row r="20" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="55"/>
-    </row>
-    <row r="21" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="55"/>
-    </row>
-    <row r="22" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="55"/>
-    </row>
-    <row r="23" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="55"/>
-    </row>
-    <row r="24" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="55"/>
-    </row>
-    <row r="25" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="55"/>
-    </row>
-    <row r="26" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="55"/>
-    </row>
-    <row r="27" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="55"/>
-    </row>
-    <row r="28" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="55"/>
-    </row>
-    <row r="29" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="55"/>
-    </row>
-    <row r="30" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="55"/>
-    </row>
-    <row r="31" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="55"/>
-    </row>
-    <row r="32" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="55"/>
-    </row>
-    <row r="33" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="55"/>
-    </row>
-    <row r="34" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="55"/>
-    </row>
-    <row r="35" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="50"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="55"/>
-    </row>
-    <row r="36" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="50"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52"/>
-      <c r="I36" s="52"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="55"/>
-    </row>
-    <row r="37" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
-      <c r="B37" s="51"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="55"/>
-    </row>
-    <row r="38" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
-      <c r="B38" s="51"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="52"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="55"/>
-    </row>
-    <row r="39" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
-      <c r="B39" s="51"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="55"/>
-    </row>
-    <row r="40" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="54"/>
-      <c r="K40" s="55"/>
-    </row>
-    <row r="41" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="54"/>
-      <c r="K41" s="55"/>
-    </row>
-    <row r="42" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="50"/>
-      <c r="B42" s="51"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="55"/>
-    </row>
-    <row r="43" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="52"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="54"/>
-      <c r="K43" s="55"/>
-    </row>
-    <row r="44" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="50"/>
-      <c r="B44" s="51"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="54"/>
-      <c r="K44" s="55"/>
-    </row>
-    <row r="45" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="54"/>
-      <c r="K45" s="55"/>
-    </row>
-    <row r="46" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="52"/>
-      <c r="J46" s="54"/>
-      <c r="K46" s="55"/>
-    </row>
-    <row r="47" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
-      <c r="B47" s="51"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="55"/>
-    </row>
-    <row r="48" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="50"/>
-      <c r="B48" s="51"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="55"/>
-    </row>
-    <row r="49" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="50"/>
-      <c r="B49" s="51"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="54"/>
-      <c r="K49" s="55"/>
-    </row>
-    <row r="50" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="50"/>
-      <c r="B50" s="51"/>
-      <c r="C50" s="52"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="52"/>
-      <c r="J50" s="54"/>
-      <c r="K50" s="55"/>
-    </row>
-    <row r="51" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="50"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="52"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="55"/>
-    </row>
-    <row r="52" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="50"/>
-      <c r="B52" s="51"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="52"/>
-      <c r="J52" s="54"/>
-      <c r="K52" s="55"/>
-    </row>
-    <row r="53" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="50"/>
-      <c r="B53" s="51"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="50"/>
-      <c r="H53" s="50"/>
-      <c r="I53" s="50"/>
-      <c r="J53" s="54"/>
-      <c r="K53" s="55"/>
-    </row>
-    <row r="54" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="50"/>
-      <c r="B54" s="51"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="52"/>
-      <c r="H54" s="52"/>
-      <c r="I54" s="52"/>
-      <c r="J54" s="54"/>
-      <c r="K54" s="55"/>
-    </row>
-    <row r="55" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="50"/>
-      <c r="B55" s="51"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="50"/>
-      <c r="I55" s="50"/>
-      <c r="J55" s="54"/>
-      <c r="K55" s="55"/>
-    </row>
-    <row r="56" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="50"/>
-      <c r="B56" s="51"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="52"/>
-      <c r="F56" s="52"/>
-      <c r="G56" s="52"/>
-      <c r="H56" s="52"/>
-      <c r="I56" s="52"/>
-      <c r="J56" s="54"/>
-      <c r="K56" s="55"/>
-    </row>
-    <row r="57" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="50"/>
-      <c r="B57" s="51"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="54"/>
-      <c r="K57" s="55"/>
-    </row>
-    <row r="58" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="50"/>
-      <c r="B58" s="51"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="52"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="52"/>
-      <c r="J58" s="54"/>
-      <c r="K58" s="55"/>
-    </row>
-    <row r="59" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="50"/>
-      <c r="B59" s="51"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="50"/>
-      <c r="I59" s="50"/>
-      <c r="J59" s="54"/>
-      <c r="K59" s="55"/>
-    </row>
-    <row r="60" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="50"/>
-      <c r="B60" s="51"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="52"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="52"/>
-      <c r="H60" s="52"/>
-      <c r="I60" s="52"/>
-      <c r="J60" s="54"/>
-      <c r="K60" s="55"/>
-    </row>
-    <row r="61" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="50"/>
-      <c r="B61" s="51"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="53"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="54"/>
-      <c r="K61" s="55"/>
-    </row>
-    <row r="62" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="50"/>
-      <c r="B62" s="51"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="52"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-      <c r="J62" s="54"/>
-      <c r="K62" s="55"/>
-    </row>
-    <row r="63" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="50"/>
-      <c r="B63" s="51"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="53"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="50"/>
-      <c r="G63" s="50"/>
-      <c r="H63" s="50"/>
-      <c r="I63" s="50"/>
-      <c r="J63" s="54"/>
-      <c r="K63" s="55"/>
-    </row>
-    <row r="64" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="50"/>
-      <c r="B64" s="51"/>
-      <c r="C64" s="52"/>
-      <c r="D64" s="53"/>
-      <c r="E64" s="52"/>
-      <c r="F64" s="52"/>
-      <c r="G64" s="52"/>
-      <c r="H64" s="52"/>
-      <c r="I64" s="52"/>
-      <c r="J64" s="54"/>
-      <c r="K64" s="55"/>
-    </row>
-    <row r="65" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="50"/>
-      <c r="B65" s="51"/>
-      <c r="C65" s="52"/>
-      <c r="D65" s="53"/>
-      <c r="E65" s="50"/>
-      <c r="F65" s="50"/>
-      <c r="G65" s="50"/>
-      <c r="H65" s="50"/>
-      <c r="I65" s="50"/>
-      <c r="J65" s="54"/>
-      <c r="K65" s="55"/>
-    </row>
-    <row r="66" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="50"/>
-      <c r="B66" s="51"/>
-      <c r="C66" s="52"/>
-      <c r="D66" s="53"/>
-      <c r="E66" s="52"/>
-      <c r="F66" s="52"/>
-      <c r="G66" s="52"/>
-      <c r="H66" s="52"/>
-      <c r="I66" s="52"/>
-      <c r="J66" s="54"/>
-      <c r="K66" s="55"/>
-    </row>
-    <row r="67" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="50"/>
-      <c r="B67" s="51"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="53"/>
-      <c r="E67" s="50"/>
-      <c r="F67" s="50"/>
-      <c r="G67" s="50"/>
-      <c r="H67" s="50"/>
-      <c r="I67" s="50"/>
-      <c r="J67" s="54"/>
-      <c r="K67" s="55"/>
-    </row>
-    <row r="68" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="50"/>
-      <c r="B68" s="51"/>
-      <c r="C68" s="52"/>
-      <c r="D68" s="53"/>
-      <c r="E68" s="52"/>
-      <c r="F68" s="52"/>
-      <c r="G68" s="52"/>
-      <c r="H68" s="52"/>
-      <c r="I68" s="52"/>
-      <c r="J68" s="54"/>
-      <c r="K68" s="55"/>
-    </row>
-    <row r="69" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="50"/>
-      <c r="B69" s="51"/>
-      <c r="C69" s="52"/>
-      <c r="D69" s="53"/>
-      <c r="E69" s="50"/>
-      <c r="F69" s="50"/>
-      <c r="G69" s="50"/>
-      <c r="H69" s="50"/>
-      <c r="I69" s="50"/>
-      <c r="J69" s="54"/>
-      <c r="K69" s="55"/>
-    </row>
-    <row r="70" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="50"/>
-      <c r="B70" s="51"/>
-      <c r="C70" s="52"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="52"/>
-      <c r="F70" s="52"/>
-      <c r="G70" s="52"/>
-      <c r="H70" s="52"/>
-      <c r="I70" s="52"/>
-      <c r="J70" s="54"/>
-      <c r="K70" s="55"/>
-    </row>
-    <row r="71" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="50"/>
-      <c r="B71" s="51"/>
-      <c r="C71" s="52"/>
-      <c r="D71" s="53"/>
-      <c r="E71" s="50"/>
-      <c r="F71" s="50"/>
-      <c r="G71" s="50"/>
-      <c r="H71" s="50"/>
-      <c r="I71" s="50"/>
-      <c r="J71" s="54"/>
-      <c r="K71" s="55"/>
-    </row>
-    <row r="72" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="50"/>
-      <c r="B72" s="51"/>
-      <c r="C72" s="52"/>
-      <c r="D72" s="53"/>
-      <c r="E72" s="52"/>
-      <c r="F72" s="52"/>
-      <c r="G72" s="52"/>
-      <c r="H72" s="52"/>
-      <c r="I72" s="52"/>
-      <c r="J72" s="54"/>
-      <c r="K72" s="55"/>
-    </row>
-    <row r="73" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="50"/>
-      <c r="B73" s="51"/>
-      <c r="C73" s="52"/>
-      <c r="D73" s="53"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="50"/>
-      <c r="H73" s="50"/>
-      <c r="I73" s="50"/>
-      <c r="J73" s="54"/>
-      <c r="K73" s="55"/>
-    </row>
-    <row r="74" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="50"/>
-      <c r="B74" s="51"/>
-      <c r="C74" s="52"/>
-      <c r="D74" s="53"/>
-      <c r="E74" s="52"/>
-      <c r="F74" s="52"/>
-      <c r="G74" s="52"/>
-      <c r="H74" s="52"/>
-      <c r="I74" s="52"/>
-      <c r="J74" s="54"/>
-      <c r="K74" s="55"/>
-    </row>
-    <row r="75" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="50"/>
-      <c r="B75" s="51"/>
-      <c r="C75" s="52"/>
-      <c r="D75" s="53"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="50"/>
-      <c r="G75" s="50"/>
-      <c r="H75" s="50"/>
-      <c r="I75" s="50"/>
-      <c r="J75" s="54"/>
-      <c r="K75" s="55"/>
-    </row>
-    <row r="76" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="43"/>
-      <c r="B76" s="44"/>
-      <c r="C76" s="45"/>
-      <c r="D76" s="46"/>
-      <c r="E76" s="45"/>
-      <c r="F76" s="45"/>
-      <c r="G76" s="45"/>
-      <c r="H76" s="45"/>
-      <c r="I76" s="45"/>
-      <c r="J76" s="47"/>
-      <c r="K76" s="48"/>
-    </row>
-    <row r="77" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="43"/>
-      <c r="B77" s="44"/>
-      <c r="C77" s="45"/>
-      <c r="D77" s="46"/>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
-      <c r="H77" s="43"/>
-      <c r="I77" s="43"/>
-      <c r="J77" s="47"/>
-      <c r="K77" s="48"/>
-    </row>
-    <row r="78" spans="1:11" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="43"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="46"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="45"/>
-      <c r="H78" s="45"/>
-      <c r="I78" s="45"/>
-      <c r="J78" s="47"/>
-      <c r="K78" s="48"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="42"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="28"/>
+    </row>
+    <row r="6" spans="1:14" s="31" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" s="38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="55">
+        <v>7</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" s="52">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="52"/>
+    </row>
+    <row r="9" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="52"/>
+    </row>
+    <row r="10" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="52"/>
+    </row>
+    <row r="11" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="52"/>
+    </row>
+    <row r="12" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="52"/>
+    </row>
+    <row r="13" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="52"/>
+    </row>
+    <row r="14" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="52"/>
+    </row>
+    <row r="15" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="52"/>
+    </row>
+    <row r="16" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="52"/>
+    </row>
+    <row r="17" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="47"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="52"/>
+    </row>
+    <row r="18" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="52"/>
+    </row>
+    <row r="19" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="52"/>
+    </row>
+    <row r="20" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="52"/>
+    </row>
+    <row r="21" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="47"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="52"/>
+    </row>
+    <row r="22" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="52"/>
+    </row>
+    <row r="23" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="47"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="52"/>
+    </row>
+    <row r="24" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="52"/>
+    </row>
+    <row r="25" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="47"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="52"/>
+    </row>
+    <row r="26" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="47"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="52"/>
+    </row>
+    <row r="27" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="47"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="52"/>
+    </row>
+    <row r="28" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="47"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="52"/>
+    </row>
+    <row r="29" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="47"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="52"/>
+    </row>
+    <row r="30" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="52"/>
+    </row>
+    <row r="31" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="52"/>
+    </row>
+    <row r="32" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="47"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="51"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="52"/>
+    </row>
+    <row r="33" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="51"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="52"/>
+    </row>
+    <row r="34" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="47"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="52"/>
+    </row>
+    <row r="35" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="47"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="52"/>
+    </row>
+    <row r="36" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="47"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="52"/>
+    </row>
+    <row r="37" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="47"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="47"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="52"/>
+    </row>
+    <row r="38" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="47"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="52"/>
+    </row>
+    <row r="39" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="47"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="52"/>
+    </row>
+    <row r="40" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="52"/>
+    </row>
+    <row r="41" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="47"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="51"/>
+      <c r="M41" s="51"/>
+      <c r="N41" s="52"/>
+    </row>
+    <row r="42" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="51"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="52"/>
+    </row>
+    <row r="43" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="47"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="51"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="52"/>
+    </row>
+    <row r="44" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="47"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="52"/>
+    </row>
+    <row r="45" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="47"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="51"/>
+      <c r="M45" s="51"/>
+      <c r="N45" s="52"/>
+    </row>
+    <row r="46" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="47"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+      <c r="L46" s="51"/>
+      <c r="M46" s="51"/>
+      <c r="N46" s="52"/>
+    </row>
+    <row r="47" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="47"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="52"/>
+    </row>
+    <row r="48" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="47"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="49"/>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="51"/>
+      <c r="N48" s="52"/>
+    </row>
+    <row r="49" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="47"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="47"/>
+      <c r="J49" s="47"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="51"/>
+      <c r="M49" s="51"/>
+      <c r="N49" s="52"/>
+    </row>
+    <row r="50" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="47"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="51"/>
+      <c r="M50" s="51"/>
+      <c r="N50" s="52"/>
+    </row>
+    <row r="51" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="47"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="47"/>
+      <c r="I51" s="47"/>
+      <c r="J51" s="47"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="51"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="52"/>
+    </row>
+    <row r="52" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="47"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="49"/>
+      <c r="J52" s="49"/>
+      <c r="K52" s="49"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="52"/>
+    </row>
+    <row r="53" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="47"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+      <c r="I53" s="47"/>
+      <c r="J53" s="47"/>
+      <c r="K53" s="47"/>
+      <c r="L53" s="51"/>
+      <c r="M53" s="51"/>
+      <c r="N53" s="52"/>
+    </row>
+    <row r="54" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="47"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="49"/>
+      <c r="L54" s="51"/>
+      <c r="M54" s="51"/>
+      <c r="N54" s="52"/>
+    </row>
+    <row r="55" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="47"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="47"/>
+      <c r="I55" s="47"/>
+      <c r="J55" s="47"/>
+      <c r="K55" s="47"/>
+      <c r="L55" s="51"/>
+      <c r="M55" s="51"/>
+      <c r="N55" s="52"/>
+    </row>
+    <row r="56" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="47"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
+      <c r="L56" s="51"/>
+      <c r="M56" s="51"/>
+      <c r="N56" s="52"/>
+    </row>
+    <row r="57" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="47"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="47"/>
+      <c r="J57" s="47"/>
+      <c r="K57" s="47"/>
+      <c r="L57" s="51"/>
+      <c r="M57" s="51"/>
+      <c r="N57" s="52"/>
+    </row>
+    <row r="58" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="47"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
+      <c r="K58" s="49"/>
+      <c r="L58" s="51"/>
+      <c r="M58" s="51"/>
+      <c r="N58" s="52"/>
+    </row>
+    <row r="59" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="47"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
+      <c r="J59" s="47"/>
+      <c r="K59" s="47"/>
+      <c r="L59" s="51"/>
+      <c r="M59" s="51"/>
+      <c r="N59" s="52"/>
+    </row>
+    <row r="60" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="47"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="49"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="49"/>
+      <c r="J60" s="49"/>
+      <c r="K60" s="49"/>
+      <c r="L60" s="51"/>
+      <c r="M60" s="51"/>
+      <c r="N60" s="52"/>
+    </row>
+    <row r="61" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="47"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="55"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="47"/>
+      <c r="L61" s="51"/>
+      <c r="M61" s="51"/>
+      <c r="N61" s="52"/>
+    </row>
+    <row r="62" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="47"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="49"/>
+      <c r="J62" s="49"/>
+      <c r="K62" s="49"/>
+      <c r="L62" s="51"/>
+      <c r="M62" s="51"/>
+      <c r="N62" s="52"/>
+    </row>
+    <row r="63" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="47"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="47"/>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
+      <c r="J63" s="47"/>
+      <c r="K63" s="47"/>
+      <c r="L63" s="51"/>
+      <c r="M63" s="51"/>
+      <c r="N63" s="52"/>
+    </row>
+    <row r="64" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="47"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="49"/>
+      <c r="J64" s="49"/>
+      <c r="K64" s="49"/>
+      <c r="L64" s="51"/>
+      <c r="M64" s="51"/>
+      <c r="N64" s="52"/>
+    </row>
+    <row r="65" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="47"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="55"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="47"/>
+      <c r="I65" s="47"/>
+      <c r="J65" s="47"/>
+      <c r="K65" s="47"/>
+      <c r="L65" s="51"/>
+      <c r="M65" s="51"/>
+      <c r="N65" s="52"/>
+    </row>
+    <row r="66" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="47"/>
+      <c r="B66" s="48"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="49"/>
+      <c r="J66" s="49"/>
+      <c r="K66" s="49"/>
+      <c r="L66" s="51"/>
+      <c r="M66" s="51"/>
+      <c r="N66" s="52"/>
+    </row>
+    <row r="67" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="47"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="49"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="47"/>
+      <c r="J67" s="47"/>
+      <c r="K67" s="47"/>
+      <c r="L67" s="51"/>
+      <c r="M67" s="51"/>
+      <c r="N67" s="52"/>
+    </row>
+    <row r="68" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="47"/>
+      <c r="B68" s="48"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="49"/>
+      <c r="J68" s="49"/>
+      <c r="K68" s="49"/>
+      <c r="L68" s="51"/>
+      <c r="M68" s="51"/>
+      <c r="N68" s="52"/>
+    </row>
+    <row r="69" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="47"/>
+      <c r="B69" s="48"/>
+      <c r="C69" s="49"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="47"/>
+      <c r="H69" s="47"/>
+      <c r="I69" s="47"/>
+      <c r="J69" s="47"/>
+      <c r="K69" s="47"/>
+      <c r="L69" s="51"/>
+      <c r="M69" s="51"/>
+      <c r="N69" s="52"/>
+    </row>
+    <row r="70" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="47"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="49"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="49"/>
+      <c r="G70" s="49"/>
+      <c r="H70" s="49"/>
+      <c r="I70" s="49"/>
+      <c r="J70" s="49"/>
+      <c r="K70" s="49"/>
+      <c r="L70" s="51"/>
+      <c r="M70" s="51"/>
+      <c r="N70" s="52"/>
+    </row>
+    <row r="71" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="47"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="49"/>
+      <c r="D71" s="50"/>
+      <c r="E71" s="55"/>
+      <c r="F71" s="47"/>
+      <c r="G71" s="47"/>
+      <c r="H71" s="47"/>
+      <c r="I71" s="47"/>
+      <c r="J71" s="47"/>
+      <c r="K71" s="47"/>
+      <c r="L71" s="51"/>
+      <c r="M71" s="51"/>
+      <c r="N71" s="52"/>
+    </row>
+    <row r="72" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="47"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="55"/>
+      <c r="F72" s="49"/>
+      <c r="G72" s="49"/>
+      <c r="H72" s="49"/>
+      <c r="I72" s="49"/>
+      <c r="J72" s="49"/>
+      <c r="K72" s="49"/>
+      <c r="L72" s="51"/>
+      <c r="M72" s="51"/>
+      <c r="N72" s="52"/>
+    </row>
+    <row r="73" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="47"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="55"/>
+      <c r="F73" s="47"/>
+      <c r="G73" s="47"/>
+      <c r="H73" s="47"/>
+      <c r="I73" s="47"/>
+      <c r="J73" s="47"/>
+      <c r="K73" s="47"/>
+      <c r="L73" s="51"/>
+      <c r="M73" s="51"/>
+      <c r="N73" s="52"/>
+    </row>
+    <row r="74" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="47"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="50"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="49"/>
+      <c r="G74" s="49"/>
+      <c r="H74" s="49"/>
+      <c r="I74" s="49"/>
+      <c r="J74" s="49"/>
+      <c r="K74" s="49"/>
+      <c r="L74" s="51"/>
+      <c r="M74" s="51"/>
+      <c r="N74" s="52"/>
+    </row>
+    <row r="75" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="47"/>
+      <c r="B75" s="48"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="55"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="47"/>
+      <c r="I75" s="47"/>
+      <c r="J75" s="47"/>
+      <c r="K75" s="47"/>
+      <c r="L75" s="51"/>
+      <c r="M75" s="51"/>
+      <c r="N75" s="52"/>
+    </row>
+    <row r="76" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="40"/>
+      <c r="B76" s="41"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="42"/>
+      <c r="J76" s="42"/>
+      <c r="K76" s="42"/>
+      <c r="L76" s="44"/>
+      <c r="M76" s="44"/>
+      <c r="N76" s="45"/>
+    </row>
+    <row r="77" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="40"/>
+      <c r="B77" s="41"/>
+      <c r="C77" s="42"/>
+      <c r="D77" s="43"/>
+      <c r="E77" s="40"/>
+      <c r="F77" s="40"/>
+      <c r="G77" s="40"/>
+      <c r="H77" s="40"/>
+      <c r="I77" s="40"/>
+      <c r="J77" s="40"/>
+      <c r="K77" s="40"/>
+      <c r="L77" s="44"/>
+      <c r="M77" s="44"/>
+      <c r="N77" s="45"/>
+    </row>
+    <row r="78" spans="1:14" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="40"/>
+      <c r="B78" s="41"/>
+      <c r="C78" s="42"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="42"/>
+      <c r="F78" s="42"/>
+      <c r="G78" s="42"/>
+      <c r="H78" s="42"/>
+      <c r="I78" s="42"/>
+      <c r="J78" s="42"/>
+      <c r="K78" s="42"/>
+      <c r="L78" s="44"/>
+      <c r="M78" s="44"/>
+      <c r="N78" s="45"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="39"/>
       <c r="B79"/>
       <c r="C79"/>
-      <c r="D79" s="36"/>
+      <c r="D79" s="33"/>
       <c r="E79"/>
       <c r="F79"/>
-      <c r="G79" s="33"/>
-      <c r="H79" s="33"/>
+      <c r="G79" s="30"/>
+      <c r="H79" s="30"/>
       <c r="I79"/>
-      <c r="J79"/>
-      <c r="K79"/>
+      <c r="J79" s="30"/>
+      <c r="K79" s="30"/>
+      <c r="L79"/>
+      <c r="M79" s="30"/>
+      <c r="N79"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3061,7 +3506,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="16.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -3103,7 +3548,7 @@
       <c r="O2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="Q2" s="22" t="s">
         <v>12</v>
       </c>
       <c r="R2" s="9"/>
@@ -3165,7 +3610,7 @@
         <f>IF(LEN($M$3)&gt;0,MID($M$3,LEN($M$3),1),0)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="57" t="s">
+      <c r="Q3" s="54" t="s">
         <v>15</v>
       </c>
       <c r="R3" s="9">
@@ -3229,7 +3674,7 @@
         <f>IF(LEN($M$3)&gt;1,MID($M$3,LEN($M$3)-1,1),0)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="57" t="s">
+      <c r="Q4" s="54" t="s">
         <v>16</v>
       </c>
       <c r="R4" s="9">
@@ -3289,7 +3734,7 @@
         <f>IF(LEN($M$3)&gt;2,MID($M$3,LEN($M$3)-2,1),0)</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="57" t="s">
+      <c r="Q5" s="54" t="s">
         <v>17</v>
       </c>
       <c r="R5" s="9">
@@ -3349,7 +3794,7 @@
         <f>IF(LEN($M$3)&gt;3,MID($M$3,LEN($M$3)-3,1),0)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="57" t="s">
+      <c r="Q6" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R6" s="9">
@@ -3409,7 +3854,7 @@
         <f>IF(LEN($M$3)&gt;4,MID($M$3,LEN($M$3)-4,1),0)</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="57" t="s">
+      <c r="Q7" s="54" t="s">
         <v>19</v>
       </c>
       <c r="R7" s="9">
@@ -3457,7 +3902,7 @@
         <f>IF(LEN($M$3)&gt;5,MID($M$3,LEN($M$3)-5,1),0)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="57" t="s">
+      <c r="Q8" s="54" t="s">
         <v>20</v>
       </c>
       <c r="R8" s="9">
@@ -3501,7 +3946,7 @@
       <c r="G9" s="2">
         <v>6</v>
       </c>
-      <c r="Q9" s="57" t="s">
+      <c r="Q9" s="54" t="s">
         <v>21</v>
       </c>
       <c r="R9" s="9">
@@ -3542,7 +3987,7 @@
       <c r="I10" t="s">
         <v>22</v>
       </c>
-      <c r="Q10" s="57" t="s">
+      <c r="Q10" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R10" s="9">
@@ -3582,7 +4027,7 @@
         <f>K7&amp;K6&amp;K5&amp;K4&amp;K3</f>
         <v>00000</v>
       </c>
-      <c r="Q11" s="57" t="s">
+      <c r="Q11" s="54" t="s">
         <v>24</v>
       </c>
       <c r="R11" s="9">
@@ -3618,7 +4063,7 @@
       <c r="G12" s="2">
         <v>9</v>
       </c>
-      <c r="Q12" s="57" t="s">
+      <c r="Q12" s="54" t="s">
         <v>25</v>
       </c>
       <c r="R12" s="9">
@@ -3654,7 +4099,7 @@
       <c r="G13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q13" s="56" t="s">
+      <c r="Q13" s="53" t="s">
         <v>26</v>
       </c>
       <c r="R13" s="9">
@@ -3690,7 +4135,7 @@
       <c r="G14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="Q14" s="56" t="s">
+      <c r="Q14" s="53" t="s">
         <v>6</v>
       </c>
       <c r="R14" s="9">
@@ -3726,7 +4171,7 @@
       <c r="G15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Q15" s="56" t="s">
+      <c r="Q15" s="53" t="s">
         <v>27</v>
       </c>
       <c r="R15" s="9">
@@ -3762,7 +4207,7 @@
       <c r="G16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="56" t="s">
+      <c r="Q16" s="53" t="s">
         <v>28</v>
       </c>
       <c r="R16" s="9">
@@ -3798,7 +4243,7 @@
       <c r="G17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Q17" s="56" t="s">
+      <c r="Q17" s="53" t="s">
         <v>29</v>
       </c>
       <c r="R17" s="9">
@@ -3834,7 +4279,7 @@
       <c r="G18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q18" s="56" t="s">
+      <c r="Q18" s="53" t="s">
         <v>30</v>
       </c>
       <c r="R18" s="9">
@@ -3870,7 +4315,7 @@
       <c r="G19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q19" s="56" t="s">
+      <c r="Q19" s="53" t="s">
         <v>31</v>
       </c>
       <c r="R19" s="9">
@@ -3906,7 +4351,7 @@
       <c r="G20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="Q20" s="56" t="s">
+      <c r="Q20" s="53" t="s">
         <v>32</v>
       </c>
       <c r="R20" s="9">
@@ -3942,7 +4387,7 @@
       <c r="G21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="Q21" s="56" t="s">
+      <c r="Q21" s="53" t="s">
         <v>33</v>
       </c>
       <c r="R21" s="9">
@@ -3978,7 +4423,7 @@
       <c r="G22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="Q22" s="56" t="s">
+      <c r="Q22" s="53" t="s">
         <v>34</v>
       </c>
       <c r="R22" s="9">
@@ -4014,7 +4459,7 @@
       <c r="G23" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="Q23" s="56" t="s">
+      <c r="Q23" s="53" t="s">
         <v>35</v>
       </c>
       <c r="R23" s="9">
@@ -4050,7 +4495,7 @@
       <c r="G24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="Q24" s="56" t="s">
+      <c r="Q24" s="53" t="s">
         <v>36</v>
       </c>
       <c r="R24" s="9">
@@ -4086,7 +4531,7 @@
       <c r="G25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="Q25" s="56" t="s">
+      <c r="Q25" s="53" t="s">
         <v>37</v>
       </c>
       <c r="R25" s="9">
@@ -4122,7 +4567,7 @@
       <c r="G26" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="Q26" s="56" t="s">
+      <c r="Q26" s="53" t="s">
         <v>38</v>
       </c>
       <c r="R26" s="9">
@@ -4147,7 +4592,7 @@
       <c r="G27" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="Q27" s="56" t="s">
+      <c r="Q27" s="53" t="s">
         <v>39</v>
       </c>
       <c r="R27" s="9">
@@ -4161,7 +4606,7 @@
       <c r="G28" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="Q28" s="56" t="s">
+      <c r="Q28" s="53" t="s">
         <v>40</v>
       </c>
       <c r="R28" s="9">
@@ -4175,7 +4620,7 @@
       <c r="G29" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="Q29" s="56" t="s">
+      <c r="Q29" s="53" t="s">
         <v>41</v>
       </c>
       <c r="R29" s="9">
@@ -4189,7 +4634,7 @@
       <c r="G30" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Q30" s="56" t="s">
+      <c r="Q30" s="53" t="s">
         <v>42</v>
       </c>
       <c r="R30" s="9">
@@ -4203,7 +4648,7 @@
       <c r="G31" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Q31" s="56" t="s">
+      <c r="Q31" s="53" t="s">
         <v>43</v>
       </c>
       <c r="R31" s="9">
@@ -4217,7 +4662,7 @@
       <c r="G32" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="Q32" s="56" t="s">
+      <c r="Q32" s="53" t="s">
         <v>44</v>
       </c>
       <c r="R32" s="9">
@@ -4272,8 +4717,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="61.7109375" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.140625" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4294,7 +4739,7 @@
       <c r="B2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4305,7 +4750,7 @@
       <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4316,7 +4761,7 @@
       <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4327,7 +4772,7 @@
       <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4338,7 +4783,7 @@
       <c r="B6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4349,7 +4794,7 @@
       <c r="B7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4360,7 +4805,7 @@
       <c r="B8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4371,7 +4816,7 @@
       <c r="B9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4382,7 +4827,7 @@
       <c r="B10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4393,7 +4838,7 @@
       <c r="B11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4404,7 +4849,7 @@
       <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4415,7 +4860,7 @@
       <c r="B13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4426,7 +4871,7 @@
       <c r="B14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4437,7 +4882,7 @@
       <c r="B15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4448,7 +4893,7 @@
       <c r="B16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4459,7 +4904,7 @@
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4470,7 +4915,7 @@
       <c r="B18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="30" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4481,7 +4926,7 @@
       <c r="B19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="30" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>